<commit_message>
ccbottlersus fix sos_maj adding
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS_SAND/Data/KPITemplateV4.4.xlsx
+++ b/Projects/CCBOTTLERSUS_SAND/Data/KPITemplateV4.4.xlsx
@@ -19,6 +19,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$I$63</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Survey!$A$1:$E$28</definedName>
   </definedNames>
@@ -676,7 +677,7 @@
     <t xml:space="preserve">exclusion_sheet</t>
   </si>
   <si>
-    <t xml:space="preserve">filter if not DP</t>
+    <t xml:space="preserve">add if not DP</t>
   </si>
   <si>
     <t xml:space="preserve">United Deliver</t>
@@ -1027,7 +1028,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1060,14 +1061,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1093,10 +1086,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1239,18 +1228,18 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.3886639676113"/>
@@ -2400,41 +2389,35 @@
       <c r="P35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="8" t="s">
+      <c r="A36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H36" s="4" t="s">
         <v>103</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="8" t="s">
+      <c r="L36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="8" t="n">
+      <c r="O36" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="100.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
@@ -3451,7 +3434,7 @@
       <c r="C68" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D68" s="10" t="s">
+      <c r="D68" s="8" t="s">
         <v>168</v>
       </c>
       <c r="F68" s="4" t="s">
@@ -3484,7 +3467,7 @@
       <c r="C69" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D69" s="10" t="s">
+      <c r="D69" s="8" t="s">
         <v>168</v>
       </c>
       <c r="F69" s="4" t="s">
@@ -3517,7 +3500,7 @@
       <c r="C70" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D70" s="10" t="s">
+      <c r="D70" s="8" t="s">
         <v>168</v>
       </c>
       <c r="F70" s="4" t="s">
@@ -3568,1060 +3551,1055 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8502024291498"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.89068825910931"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="I2" s="13" t="n">
+      <c r="I2" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="E3" s="13" t="n">
+      <c r="E3" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I3" s="13" t="n">
+      <c r="I3" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="E4" s="13" t="n">
+      <c r="E4" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I4" s="13" t="n">
+      <c r="I4" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="E5" s="13" t="n">
+      <c r="E5" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I5" s="13" t="n">
+      <c r="I5" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E6" s="13" t="n">
+      <c r="E6" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I6" s="13" t="n">
+      <c r="I6" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="E7" s="13" t="n">
+      <c r="E7" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I7" s="13" t="n">
+      <c r="I7" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="E8" s="13" t="n">
+      <c r="E8" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I8" s="13" t="n">
+      <c r="I8" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="I9" s="13" t="n">
+      <c r="F9" s="11"/>
+      <c r="I9" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="I10" s="13" t="n">
+      <c r="F10" s="11"/>
+      <c r="I10" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="I11" s="13" t="n">
+      <c r="F11" s="11"/>
+      <c r="I11" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="I12" s="13" t="n">
+      <c r="F12" s="11"/>
+      <c r="I12" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="I13" s="13" t="n">
+      <c r="F13" s="11"/>
+      <c r="I13" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="E14" s="13" t="n">
+      <c r="E14" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="F14" s="13" t="n">
+      <c r="F14" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="13" t="n">
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="I15" s="13" t="n">
+      <c r="F15" s="11"/>
+      <c r="I15" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="I16" s="13" t="n">
+      <c r="F16" s="11"/>
+      <c r="I16" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="I17" s="13" t="n">
+      <c r="F17" s="11"/>
+      <c r="I17" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="I18" s="15" t="n">
+      <c r="I18" s="13" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="I19" s="15" t="n">
+      <c r="I19" s="13" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15" t="s">
+      <c r="F20" s="13"/>
+      <c r="G20" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I20" s="15" t="n">
+      <c r="I20" s="13" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="E21" s="15" t="n">
+      <c r="E21" s="13" t="n">
         <v>18.5</v>
       </c>
-      <c r="F21" s="15"/>
-      <c r="I21" s="16" t="n">
+      <c r="F21" s="13"/>
+      <c r="I21" s="14" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="E22" s="15" t="n">
+      <c r="E22" s="13" t="n">
         <v>20</v>
       </c>
-      <c r="F22" s="15"/>
-      <c r="I22" s="16" t="n">
+      <c r="F22" s="13"/>
+      <c r="I22" s="14" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="I23" s="15" t="n">
+      <c r="F23" s="13"/>
+      <c r="I23" s="13" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="I24" s="13" t="n">
+      <c r="I24" s="11" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="E25" s="13" t="n">
+      <c r="E25" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I25" s="13" t="n">
+      <c r="I25" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="E26" s="13" t="n">
+      <c r="E26" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I26" s="13" t="n">
+      <c r="I26" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="E27" s="13" t="n">
+      <c r="E27" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I27" s="13" t="n">
+      <c r="I27" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E28" s="13" t="n">
+      <c r="E28" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I28" s="13" t="n">
+      <c r="I28" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="E29" s="13" t="n">
+      <c r="E29" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I29" s="13" t="n">
+      <c r="I29" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="E30" s="13" t="n">
+      <c r="E30" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="I30" s="13" t="n">
+      <c r="I30" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="I31" s="13" t="n">
+      <c r="I31" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="I32" s="13" t="n">
+      <c r="I32" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="I33" s="13" t="n">
+      <c r="I33" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="I34" s="13" t="n">
+      <c r="I34" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="I35" s="13" t="n">
+      <c r="I35" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="F36" s="13" t="n">
+      <c r="F36" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="I36" s="13" t="n">
+      <c r="I36" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="F37" s="13" t="n">
+      <c r="F37" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="I37" s="13" t="n">
+      <c r="I37" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="E38" s="13" t="n">
+      <c r="E38" s="11" t="n">
         <v>64</v>
       </c>
-      <c r="I38" s="13" t="n">
+      <c r="I38" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="E39" s="13" t="n">
+      <c r="E39" s="11" t="n">
         <v>59</v>
       </c>
-      <c r="I39" s="13" t="n">
+      <c r="I39" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="I40" s="13" t="n">
+      <c r="I40" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="E41" s="13" t="n">
+      <c r="E41" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="13" t="n">
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="E42" s="13" t="n">
+      <c r="E42" s="11" t="n">
         <v>33.8</v>
       </c>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="13" t="n">
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="E43" s="13" t="n">
+      <c r="E43" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="F43" s="13" t="n">
+      <c r="F43" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="I43" s="13" t="n">
+      <c r="I43" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="E44" s="13" t="n">
+      <c r="E44" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="F44" s="13" t="n">
+      <c r="F44" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="I44" s="13" t="n">
+      <c r="I44" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="19" t="n">
+      <c r="I45" s="16" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="I46" s="13" t="n">
+      <c r="I46" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="I47" s="13" t="n">
+      <c r="I47" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="I48" s="13" t="n">
+      <c r="I48" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="I49" s="13" t="n">
+      <c r="I49" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="I50" s="13" t="n">
+      <c r="I50" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="I51" s="13" t="n">
+      <c r="I51" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="F52" s="13" t="n">
+      <c r="F52" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="I52" s="13" t="n">
+      <c r="I52" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="F53" s="13" t="n">
+      <c r="F53" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="I53" s="13" t="n">
+      <c r="I53" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="F54" s="13" t="n">
+      <c r="F54" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="I54" s="13" t="n">
+      <c r="I54" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="F55" s="13" t="n">
+      <c r="F55" s="11" t="n">
         <v>24</v>
       </c>
-      <c r="I55" s="13" t="n">
+      <c r="I55" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="E56" s="13" t="n">
+      <c r="E56" s="11" t="n">
         <v>18.5</v>
       </c>
-      <c r="I56" s="13" t="n">
+      <c r="I56" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C57" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="E57" s="13" t="n">
+      <c r="E57" s="11" t="n">
         <v>23.7</v>
       </c>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="13" t="n">
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C58" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="E58" s="13" t="n">
+      <c r="E58" s="11" t="n">
         <v>33.8</v>
       </c>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="13" t="n">
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="E59" s="13" t="n">
+      <c r="E59" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="13" t="n">
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="E60" s="13" t="n">
+      <c r="E60" s="11" t="n">
         <v>33.8</v>
       </c>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="13" t="n">
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D61" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="E61" s="13" t="n">
+      <c r="E61" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="F61" s="13" t="n">
+      <c r="F61" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="I61" s="13" t="n">
+      <c r="I61" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D62" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="E62" s="13" t="n">
+      <c r="E62" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="F62" s="13" t="n">
+      <c r="F62" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="I62" s="13" t="n">
+      <c r="I62" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="I63" s="19" t="n">
+      <c r="I63" s="16" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4644,65 +4622,65 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L40" activeCellId="0" sqref="L40"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.67611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.0323886639676"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.4453441295547"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="18" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4797,7 +4775,7 @@
       <c r="E5" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="19" t="s">
         <v>222</v>
       </c>
       <c r="G5" s="0" t="s">
@@ -5216,7 +5194,7 @@
       <c r="K21" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="M21" s="23" t="s">
+      <c r="M21" s="20" t="s">
         <v>228</v>
       </c>
     </row>
@@ -5269,42 +5247,42 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.17004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.5991902834008"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="22" t="s">
         <v>181</v>
       </c>
     </row>
@@ -5312,13 +5290,13 @@
       <c r="A2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="0" t="n">
         <v>80</v>
       </c>
@@ -5344,10 +5322,10 @@
       <c r="F4" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="23" t="s">
         <v>231</v>
       </c>
-      <c r="H4" s="26"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="0" t="n">
         <v>80</v>
       </c>
@@ -5370,16 +5348,16 @@
       <c r="A6" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="24" t="s">
         <v>225</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="I6" s="28" t="n">
+      <c r="I6" s="25" t="n">
         <v>100</v>
       </c>
-      <c r="J6" s="28"/>
+      <c r="J6" s="25"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -5391,10 +5369,10 @@
       <c r="G7" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="I7" s="28" t="n">
+      <c r="I7" s="25" t="n">
         <v>51</v>
       </c>
-      <c r="J7" s="28"/>
+      <c r="J7" s="25"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -5449,27 +5427,27 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="90.1943319838057"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="91.0526315789474"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5502,19 +5480,19 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="24" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="C4" s="27" t="n">
+      <c r="C4" s="24" t="n">
         <v>141</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -5664,7 +5642,7 @@
       <c r="C14" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="24" t="s">
         <v>254</v>
       </c>
       <c r="E14" s="0" t="s">
@@ -5712,24 +5690,24 @@
       <c r="C17" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="24" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="24" t="s">
         <v>105</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="C18" s="27" t="n">
+      <c r="C18" s="24" t="n">
         <v>137</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="E18" s="27"/>
+      <c r="E18" s="24"/>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -5792,24 +5770,24 @@
       <c r="C22" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="24" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="24" t="s">
         <v>165</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="C23" s="27" t="n">
+      <c r="C23" s="24" t="n">
         <v>134</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="E23" s="27"/>
+      <c r="E23" s="24"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -5826,19 +5804,19 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="24" t="s">
         <v>263</v>
       </c>
-      <c r="C25" s="27" t="n">
+      <c r="C25" s="24" t="n">
         <v>110</v>
       </c>
-      <c r="D25" s="27" t="s">
+      <c r="D25" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="E25" s="27"/>
+      <c r="E25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -5867,7 +5845,7 @@
       <c r="C27" s="0" t="n">
         <v>118</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="19" t="s">
         <v>266</v>
       </c>
       <c r="E27" s="0" t="s">
@@ -5916,31 +5894,31 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.67611336032389"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="22" t="s">
         <v>268</v>
       </c>
     </row>
@@ -5977,15 +5955,15 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>271</v>
       </c>
     </row>

</xml_diff>